<commit_message>
Adding CG Appendix A and C
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnD'Amore\Source\Repos\ccda-search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3254756E-B5D7-45B1-A401-0C3A3E79F2DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A3D576-5464-48AC-88AB-D35409D82788}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12925,7 +12925,7 @@
         <v>836</v>
       </c>
       <c r="G194" t="str">
-        <f t="shared" ref="G194:G257" si="12">E194&amp;"-"&amp;F194</f>
+        <f t="shared" ref="G194:G216" si="12">E194&amp;"-"&amp;F194</f>
         <v>831-836</v>
       </c>
       <c r="H194" t="s">
@@ -12938,7 +12938,7 @@
         <v>553</v>
       </c>
       <c r="K194" t="str">
-        <f t="shared" ref="K194:K257" si="13">B194&amp;" "&amp;D194&amp;" "&amp;J194</f>
+        <f t="shared" ref="K194:K240" si="13">B194&amp;" "&amp;D194&amp;" "&amp;J194</f>
         <v>Smoking Status - Meaningful Use  2.16.840.1.113883.10.20.22.4.78 CONF:1098-14806;CONF:1098-14807;CONF:1098-14815;CONF:1098-14816;CONF:1098-32573;CONF:1098-32401;CONF:1098-19170;CONF:1098-31039;CONF:1098-32157;CONF:1098-14809;CONF:1098-19116;CONF:1098-31928;CONF:1098-32894;CONF:1098-32895;CONF:1098-32896;CONF:1098-32897;CONF:1098-14810;CONF:1098-14817;CONF:1098-31019;CONF:1098-31148</v>
       </c>
       <c r="M194" t="str">
@@ -14744,8 +14744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BAB6032-5C0F-4521-92AE-0A81726C47DD}">
   <dimension ref="A1:I240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="I127" sqref="I127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D218" sqref="D218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updating individual page header info
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Repos\ccda-search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F436ABB-7915-4E93-822D-5EC39CEBDC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4AABBD-354C-4B35-9C52-711CA3E4E557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="pub_releases_dates" sheetId="3" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
     <sheet name="2022_New_Pages" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4518" uniqueCount="1869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4733" uniqueCount="1869">
   <si>
     <t>Template_Type</t>
   </si>
@@ -6504,8 +6505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E177" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M240"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G216" sqref="D2:G216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35461,4 +35462,3245 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16808B2F-A187-4C43-8DFB-56A6B23E538C}">
+  <dimension ref="H16:K230"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16:K230"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="16" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <v>87</v>
+      </c>
+      <c r="J16">
+        <v>101</v>
+      </c>
+      <c r="K16" t="str">
+        <f>"{ 'index':'"&amp;H16&amp;"', 'start':"&amp;I16&amp;", 'end':"&amp;J16&amp;"},"</f>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.15', 'start':87, 'end':101},</v>
+      </c>
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>101</v>
+      </c>
+      <c r="J17">
+        <v>117</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" ref="K17:K80" si="0">"{ 'index':'"&amp;H17&amp;"', 'start':"&amp;I17&amp;", 'end':"&amp;J17&amp;"},"</f>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.4', 'start':101, 'end':117},</v>
+      </c>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18">
+        <v>117</v>
+      </c>
+      <c r="J18">
+        <v>127</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.2', 'start':117, 'end':127},</v>
+      </c>
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19">
+        <v>127</v>
+      </c>
+      <c r="J19">
+        <v>139</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.5', 'start':127, 'end':139},</v>
+      </c>
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20">
+        <v>139</v>
+      </c>
+      <c r="J20">
+        <v>153</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.8', 'start':139, 'end':153},</v>
+      </c>
+    </row>
+    <row r="21" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21">
+        <v>153</v>
+      </c>
+      <c r="J21">
+        <v>164</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.3', 'start':153, 'end':164},</v>
+      </c>
+    </row>
+    <row r="22" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22">
+        <v>164</v>
+      </c>
+      <c r="J22">
+        <v>176</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.7', 'start':164, 'end':176},</v>
+      </c>
+    </row>
+    <row r="23" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23">
+        <v>176</v>
+      </c>
+      <c r="J23">
+        <v>192</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.6', 'start':176, 'end':192},</v>
+      </c>
+    </row>
+    <row r="24" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24">
+        <v>192</v>
+      </c>
+      <c r="J24">
+        <v>202</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.9', 'start':192, 'end':202},</v>
+      </c>
+    </row>
+    <row r="25" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25">
+        <v>202</v>
+      </c>
+      <c r="J25">
+        <v>215</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.14', 'start':202, 'end':215},</v>
+      </c>
+    </row>
+    <row r="26" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26">
+        <v>215</v>
+      </c>
+      <c r="J26">
+        <v>229</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.13', 'start':215, 'end':229},</v>
+      </c>
+    </row>
+    <row r="27" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27">
+        <v>229</v>
+      </c>
+      <c r="J27">
+        <v>233</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.10', 'start':229, 'end':233},</v>
+      </c>
+    </row>
+    <row r="28" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28">
+        <v>255</v>
+      </c>
+      <c r="J28">
+        <v>257</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.43', 'start':255, 'end':257},</v>
+      </c>
+    </row>
+    <row r="29" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29">
+        <v>257</v>
+      </c>
+      <c r="J29">
+        <v>258</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.44', 'start':257, 'end':258},</v>
+      </c>
+    </row>
+    <row r="30" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>38</v>
+      </c>
+      <c r="I30">
+        <v>258</v>
+      </c>
+      <c r="J30">
+        <v>260</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.21', 'start':258, 'end':260},</v>
+      </c>
+    </row>
+    <row r="31" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31">
+        <v>260</v>
+      </c>
+      <c r="J31">
+        <v>263</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.21.1', 'start':260, 'end':263},</v>
+      </c>
+    </row>
+    <row r="32" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32">
+        <v>263</v>
+      </c>
+      <c r="J32">
+        <v>264</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.6', 'start':263, 'end':264},</v>
+      </c>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>44</v>
+      </c>
+      <c r="I33">
+        <v>264</v>
+      </c>
+      <c r="J33">
+        <v>266</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.6.1', 'start':264, 'end':266},</v>
+      </c>
+    </row>
+    <row r="34" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I34">
+        <v>266</v>
+      </c>
+      <c r="J34">
+        <v>269</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.25', 'start':266, 'end':269},</v>
+      </c>
+    </row>
+    <row r="35" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35">
+        <v>269</v>
+      </c>
+      <c r="J35">
+        <v>270</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.9', 'start':269, 'end':270},</v>
+      </c>
+    </row>
+    <row r="36" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36">
+        <v>270</v>
+      </c>
+      <c r="J36">
+        <v>272</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.8', 'start':270, 'end':272},</v>
+      </c>
+    </row>
+    <row r="37" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I37">
+        <v>272</v>
+      </c>
+      <c r="J37">
+        <v>273</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.13', 'start':272, 'end':273},</v>
+      </c>
+    </row>
+    <row r="38" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38">
+        <v>273</v>
+      </c>
+      <c r="J38">
+        <v>274</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'1.3.6.1.4.1.19376.1.5.3.1.1.13.2.1', 'start':273, 'end':274},</v>
+      </c>
+    </row>
+    <row r="39" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>56</v>
+      </c>
+      <c r="I39">
+        <v>274</v>
+      </c>
+      <c r="J39">
+        <v>276</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.37', 'start':274, 'end':276},</v>
+      </c>
+    </row>
+    <row r="40" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>58</v>
+      </c>
+      <c r="I40">
+        <v>276</v>
+      </c>
+      <c r="J40">
+        <v>278</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.64', 'start':276, 'end':278},</v>
+      </c>
+    </row>
+    <row r="41" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>60</v>
+      </c>
+      <c r="I41">
+        <v>278</v>
+      </c>
+      <c r="J41">
+        <v>281</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.1.1', 'start':278, 'end':281},</v>
+      </c>
+    </row>
+    <row r="42" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>654</v>
+      </c>
+      <c r="I42">
+        <v>281</v>
+      </c>
+      <c r="J42">
+        <v>283</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.24', 'start':281, 'end':283},</v>
+      </c>
+    </row>
+    <row r="43" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>62</v>
+      </c>
+      <c r="I43">
+        <v>283</v>
+      </c>
+      <c r="J43">
+        <v>284</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'1.3.6.1.4.1.19376.1.5.3.1.3.33', 'start':283, 'end':284},</v>
+      </c>
+    </row>
+    <row r="44" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44">
+        <v>284</v>
+      </c>
+      <c r="J44">
+        <v>286</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.11', 'start':284, 'end':286},</v>
+      </c>
+    </row>
+    <row r="45" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>67</v>
+      </c>
+      <c r="I45">
+        <v>286</v>
+      </c>
+      <c r="J45">
+        <v>289</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.11.1', 'start':286, 'end':289},</v>
+      </c>
+    </row>
+    <row r="46" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>69</v>
+      </c>
+      <c r="I46">
+        <v>289</v>
+      </c>
+      <c r="J46">
+        <v>290</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.22', 'start':289, 'end':290},</v>
+      </c>
+    </row>
+    <row r="47" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>71</v>
+      </c>
+      <c r="I47">
+        <v>290</v>
+      </c>
+      <c r="J47">
+        <v>292</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.22.1', 'start':290, 'end':292},</v>
+      </c>
+    </row>
+    <row r="48" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>73</v>
+      </c>
+      <c r="I48">
+        <v>292</v>
+      </c>
+      <c r="J48">
+        <v>294</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.15', 'start':292, 'end':294},</v>
+      </c>
+    </row>
+    <row r="49" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>75</v>
+      </c>
+      <c r="I49">
+        <v>294</v>
+      </c>
+      <c r="J49">
+        <v>296</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.3', 'start':294, 'end':296},</v>
+      </c>
+    </row>
+    <row r="50" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>77</v>
+      </c>
+      <c r="I50">
+        <v>296</v>
+      </c>
+      <c r="J50">
+        <v>297</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.1.2', 'start':296, 'end':297},</v>
+      </c>
+    </row>
+    <row r="51" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>79</v>
+      </c>
+      <c r="I51">
+        <v>297</v>
+      </c>
+      <c r="J51">
+        <v>302</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.14', 'start':297, 'end':302},</v>
+      </c>
+    </row>
+    <row r="52" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>81</v>
+      </c>
+      <c r="I52">
+        <v>302</v>
+      </c>
+      <c r="J52">
+        <v>303</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.2.5', 'start':302, 'end':303},</v>
+      </c>
+    </row>
+    <row r="53" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>83</v>
+      </c>
+      <c r="I53">
+        <v>303</v>
+      </c>
+      <c r="J53">
+        <v>305</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.60', 'start':303, 'end':305},</v>
+      </c>
+    </row>
+    <row r="54" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>85</v>
+      </c>
+      <c r="I54">
+        <v>305</v>
+      </c>
+      <c r="J54">
+        <v>308</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.58', 'start':305, 'end':308},</v>
+      </c>
+    </row>
+    <row r="55" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>87</v>
+      </c>
+      <c r="I55">
+        <v>308</v>
+      </c>
+      <c r="J55">
+        <v>310</v>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.61', 'start':308, 'end':310},</v>
+      </c>
+    </row>
+    <row r="56" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>89</v>
+      </c>
+      <c r="I56">
+        <v>310</v>
+      </c>
+      <c r="J56">
+        <v>312</v>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'1.3.6.1.4.1.19376.1.5.3.1.3.4', 'start':310, 'end':312},</v>
+      </c>
+    </row>
+    <row r="57" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>91</v>
+      </c>
+      <c r="I57">
+        <v>312</v>
+      </c>
+      <c r="J57">
+        <v>314</v>
+      </c>
+      <c r="K57" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.42', 'start':312, 'end':314},</v>
+      </c>
+    </row>
+    <row r="58" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>93</v>
+      </c>
+      <c r="I58">
+        <v>314</v>
+      </c>
+      <c r="J58">
+        <v>315</v>
+      </c>
+      <c r="K58" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'1.3.6.1.4.1.19376.1.5.3.1.3.5', 'start':314, 'end':315},</v>
+      </c>
+    </row>
+    <row r="59" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>95</v>
+      </c>
+      <c r="I59">
+        <v>315</v>
+      </c>
+      <c r="J59">
+        <v>316</v>
+      </c>
+      <c r="K59" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.41', 'start':315, 'end':316},</v>
+      </c>
+    </row>
+    <row r="60" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>97</v>
+      </c>
+      <c r="I60">
+        <v>316</v>
+      </c>
+      <c r="J60">
+        <v>318</v>
+      </c>
+      <c r="K60" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'1.3.6.1.4.1.19376.1.5.3.1.3.26', 'start':316, 'end':318},</v>
+      </c>
+    </row>
+    <row r="61" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
+        <v>99</v>
+      </c>
+      <c r="I61">
+        <v>318</v>
+      </c>
+      <c r="J61">
+        <v>320</v>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.16', 'start':318, 'end':320},</v>
+      </c>
+    </row>
+    <row r="62" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>101</v>
+      </c>
+      <c r="I62">
+        <v>320</v>
+      </c>
+      <c r="J62">
+        <v>321</v>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.2', 'start':320, 'end':321},</v>
+      </c>
+    </row>
+    <row r="63" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>103</v>
+      </c>
+      <c r="I63">
+        <v>321</v>
+      </c>
+      <c r="J63">
+        <v>325</v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.2.1', 'start':321, 'end':325},</v>
+      </c>
+    </row>
+    <row r="64" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H64" t="s">
+        <v>105</v>
+      </c>
+      <c r="I64">
+        <v>325</v>
+      </c>
+      <c r="J64">
+        <v>326</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.33', 'start':325, 'end':326},</v>
+      </c>
+    </row>
+    <row r="65" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
+        <v>107</v>
+      </c>
+      <c r="I65">
+        <v>326</v>
+      </c>
+      <c r="J65">
+        <v>328</v>
+      </c>
+      <c r="K65" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.45', 'start':326, 'end':328},</v>
+      </c>
+    </row>
+    <row r="66" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>109</v>
+      </c>
+      <c r="I66">
+        <v>328</v>
+      </c>
+      <c r="J66">
+        <v>330</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.21.2.3', 'start':328, 'end':330},</v>
+      </c>
+    </row>
+    <row r="67" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
+        <v>111</v>
+      </c>
+      <c r="I67">
+        <v>330</v>
+      </c>
+      <c r="J67">
+        <v>331</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.39', 'start':330, 'end':331},</v>
+      </c>
+    </row>
+    <row r="68" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>113</v>
+      </c>
+      <c r="I68">
+        <v>331</v>
+      </c>
+      <c r="J68">
+        <v>334</v>
+      </c>
+      <c r="K68" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.23', 'start':331, 'end':334},</v>
+      </c>
+    </row>
+    <row r="69" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H69" t="s">
+        <v>115</v>
+      </c>
+      <c r="I69">
+        <v>334</v>
+      </c>
+      <c r="J69">
+        <v>337</v>
+      </c>
+      <c r="K69" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.38', 'start':334, 'end':337},</v>
+      </c>
+    </row>
+    <row r="70" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>117</v>
+      </c>
+      <c r="I70">
+        <v>337</v>
+      </c>
+      <c r="J70">
+        <v>338</v>
+      </c>
+      <c r="K70" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.1', 'start':337, 'end':338},</v>
+      </c>
+    </row>
+    <row r="71" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
+        <v>119</v>
+      </c>
+      <c r="I71">
+        <v>338</v>
+      </c>
+      <c r="J71">
+        <v>340</v>
+      </c>
+      <c r="K71" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.1.1', 'start':338, 'end':340},</v>
+      </c>
+    </row>
+    <row r="72" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>121</v>
+      </c>
+      <c r="I72">
+        <v>340</v>
+      </c>
+      <c r="J72">
+        <v>345</v>
+      </c>
+      <c r="K72" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.56', 'start':340, 'end':345},</v>
+      </c>
+    </row>
+    <row r="73" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I73">
+        <v>345</v>
+      </c>
+      <c r="J73">
+        <v>347</v>
+      </c>
+      <c r="K73" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.57', 'start':345, 'end':347},</v>
+      </c>
+    </row>
+    <row r="74" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H74" t="s">
+        <v>125</v>
+      </c>
+      <c r="I74">
+        <v>347</v>
+      </c>
+      <c r="J74">
+        <v>348</v>
+      </c>
+      <c r="K74" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.21.2.1', 'start':347, 'end':348},</v>
+      </c>
+    </row>
+    <row r="75" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>127</v>
+      </c>
+      <c r="I75">
+        <v>348</v>
+      </c>
+      <c r="J75">
+        <v>349</v>
+      </c>
+      <c r="K75" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.4', 'start':348, 'end':349},</v>
+      </c>
+    </row>
+    <row r="76" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
+        <v>129</v>
+      </c>
+      <c r="I76">
+        <v>349</v>
+      </c>
+      <c r="J76">
+        <v>350</v>
+      </c>
+      <c r="K76" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.7.12', 'start':349, 'end':350},</v>
+      </c>
+    </row>
+    <row r="77" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>131</v>
+      </c>
+      <c r="I77">
+        <v>350</v>
+      </c>
+      <c r="J77">
+        <v>352</v>
+      </c>
+      <c r="K77" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.7.14', 'start':350, 'end':352},</v>
+      </c>
+    </row>
+    <row r="78" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>133</v>
+      </c>
+      <c r="I78">
+        <v>352</v>
+      </c>
+      <c r="J78">
+        <v>353</v>
+      </c>
+      <c r="K78" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.20', 'start':352, 'end':353},</v>
+      </c>
+    </row>
+    <row r="79" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H79" t="s">
+        <v>135</v>
+      </c>
+      <c r="I79">
+        <v>353</v>
+      </c>
+      <c r="J79">
+        <v>356</v>
+      </c>
+      <c r="K79" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.18', 'start':353, 'end':356},</v>
+      </c>
+    </row>
+    <row r="80" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>137</v>
+      </c>
+      <c r="I80">
+        <v>356</v>
+      </c>
+      <c r="J80">
+        <v>360</v>
+      </c>
+      <c r="K80" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.2.10', 'start':356, 'end':360},</v>
+      </c>
+    </row>
+    <row r="81" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>139</v>
+      </c>
+      <c r="I81">
+        <v>360</v>
+      </c>
+      <c r="J81">
+        <v>365</v>
+      </c>
+      <c r="K81" t="str">
+        <f t="shared" ref="K81:K144" si="1">"{ 'index':'"&amp;H81&amp;"', 'start':"&amp;I81&amp;", 'end':"&amp;J81&amp;"},"</f>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.10', 'start':360, 'end':365},</v>
+      </c>
+    </row>
+    <row r="82" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>141</v>
+      </c>
+      <c r="I82">
+        <v>365</v>
+      </c>
+      <c r="J82">
+        <v>367</v>
+      </c>
+      <c r="K82" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.30', 'start':365, 'end':367},</v>
+      </c>
+    </row>
+    <row r="83" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>143</v>
+      </c>
+      <c r="I83">
+        <v>367</v>
+      </c>
+      <c r="J83">
+        <v>368</v>
+      </c>
+      <c r="K83" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.35', 'start':367, 'end':368},</v>
+      </c>
+    </row>
+    <row r="84" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H84" t="s">
+        <v>145</v>
+      </c>
+      <c r="I84">
+        <v>368</v>
+      </c>
+      <c r="J84">
+        <v>370</v>
+      </c>
+      <c r="K84" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.36', 'start':368, 'end':370},</v>
+      </c>
+    </row>
+    <row r="85" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>147</v>
+      </c>
+      <c r="I85">
+        <v>370</v>
+      </c>
+      <c r="J85">
+        <v>372</v>
+      </c>
+      <c r="K85" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.34', 'start':370, 'end':372},</v>
+      </c>
+    </row>
+    <row r="86" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>149</v>
+      </c>
+      <c r="I86">
+        <v>372</v>
+      </c>
+      <c r="J86">
+        <v>374</v>
+      </c>
+      <c r="K86" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.5', 'start':372, 'end':374},</v>
+      </c>
+    </row>
+    <row r="87" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
+        <v>151</v>
+      </c>
+      <c r="I87">
+        <v>374</v>
+      </c>
+      <c r="J87">
+        <v>378</v>
+      </c>
+      <c r="K87" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.5.1', 'start':374, 'end':378},</v>
+      </c>
+    </row>
+    <row r="88" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>153</v>
+      </c>
+      <c r="I88">
+        <v>378</v>
+      </c>
+      <c r="J88">
+        <v>380</v>
+      </c>
+      <c r="K88" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.27', 'start':378, 'end':380},</v>
+      </c>
+    </row>
+    <row r="89" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>155</v>
+      </c>
+      <c r="I89">
+        <v>380</v>
+      </c>
+      <c r="J89">
+        <v>381</v>
+      </c>
+      <c r="K89" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.18.2.12', 'start':380, 'end':381},</v>
+      </c>
+    </row>
+    <row r="90" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H90" t="s">
+        <v>157</v>
+      </c>
+      <c r="I90">
+        <v>381</v>
+      </c>
+      <c r="J90">
+        <v>382</v>
+      </c>
+      <c r="K90" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.18.2.9', 'start':381, 'end':382},</v>
+      </c>
+    </row>
+    <row r="91" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>159</v>
+      </c>
+      <c r="I91">
+        <v>382</v>
+      </c>
+      <c r="J91">
+        <v>384</v>
+      </c>
+      <c r="K91" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.28', 'start':382, 'end':384},</v>
+      </c>
+    </row>
+    <row r="92" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>161</v>
+      </c>
+      <c r="I92">
+        <v>384</v>
+      </c>
+      <c r="J92">
+        <v>385</v>
+      </c>
+      <c r="K92" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.40', 'start':384, 'end':385},</v>
+      </c>
+    </row>
+    <row r="93" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>163</v>
+      </c>
+      <c r="I93">
+        <v>385</v>
+      </c>
+      <c r="J93">
+        <v>387</v>
+      </c>
+      <c r="K93" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.29', 'start':385, 'end':387},</v>
+      </c>
+    </row>
+    <row r="94" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H94" t="s">
+        <v>165</v>
+      </c>
+      <c r="I94">
+        <v>387</v>
+      </c>
+      <c r="J94">
+        <v>388</v>
+      </c>
+      <c r="K94" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.31', 'start':387, 'end':388},</v>
+      </c>
+    </row>
+    <row r="95" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H95" t="s">
+        <v>167</v>
+      </c>
+      <c r="I95">
+        <v>388</v>
+      </c>
+      <c r="J95">
+        <v>390</v>
+      </c>
+      <c r="K95" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.7', 'start':388, 'end':390},</v>
+      </c>
+    </row>
+    <row r="96" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H96" t="s">
+        <v>169</v>
+      </c>
+      <c r="I96">
+        <v>390</v>
+      </c>
+      <c r="J96">
+        <v>393</v>
+      </c>
+      <c r="K96" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.7.1', 'start':390, 'end':393},</v>
+      </c>
+    </row>
+    <row r="97" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H97" t="s">
+        <v>171</v>
+      </c>
+      <c r="I97">
+        <v>393</v>
+      </c>
+      <c r="J97">
+        <v>395</v>
+      </c>
+      <c r="K97" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'1.3.6.1.4.1.19376.1.5.3.1.3.1', 'start':393, 'end':395},</v>
+      </c>
+    </row>
+    <row r="98" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H98" t="s">
+        <v>173</v>
+      </c>
+      <c r="I98">
+        <v>395</v>
+      </c>
+      <c r="J98">
+        <v>397</v>
+      </c>
+      <c r="K98" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.12', 'start':395, 'end':397},</v>
+      </c>
+    </row>
+    <row r="99" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H99" t="s">
+        <v>175</v>
+      </c>
+      <c r="I99">
+        <v>397</v>
+      </c>
+      <c r="J99">
+        <v>399</v>
+      </c>
+      <c r="K99" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.3', 'start':397, 'end':399},</v>
+      </c>
+    </row>
+    <row r="100" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H100" t="s">
+        <v>177</v>
+      </c>
+      <c r="I100">
+        <v>399</v>
+      </c>
+      <c r="J100">
+        <v>401</v>
+      </c>
+      <c r="K100" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.3.1', 'start':399, 'end':401},</v>
+      </c>
+    </row>
+    <row r="101" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H101" t="s">
+        <v>179</v>
+      </c>
+      <c r="I101">
+        <v>401</v>
+      </c>
+      <c r="J101">
+        <v>403</v>
+      </c>
+      <c r="K101" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'1.3.6.1.4.1.19376.1.5.3.1.3.18', 'start':401, 'end':403},</v>
+      </c>
+    </row>
+    <row r="102" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H102" t="s">
+        <v>181</v>
+      </c>
+      <c r="I102">
+        <v>403</v>
+      </c>
+      <c r="J102">
+        <v>407</v>
+      </c>
+      <c r="K102" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.17', 'start':403, 'end':407},</v>
+      </c>
+    </row>
+    <row r="103" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H103" t="s">
+        <v>183</v>
+      </c>
+      <c r="I103">
+        <v>407</v>
+      </c>
+      <c r="J103">
+        <v>408</v>
+      </c>
+      <c r="K103" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.21.2.2', 'start':407, 'end':408},</v>
+      </c>
+    </row>
+    <row r="104" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H104" t="s">
+        <v>185</v>
+      </c>
+      <c r="I104">
+        <v>408</v>
+      </c>
+      <c r="J104">
+        <v>409</v>
+      </c>
+      <c r="K104" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.26', 'start':408, 'end':409},</v>
+      </c>
+    </row>
+    <row r="105" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H105" t="s">
+        <v>187</v>
+      </c>
+      <c r="I105">
+        <v>409</v>
+      </c>
+      <c r="J105">
+        <v>411</v>
+      </c>
+      <c r="K105" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.7.13', 'start':409, 'end':411},</v>
+      </c>
+    </row>
+    <row r="106" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>189</v>
+      </c>
+      <c r="I106">
+        <v>411</v>
+      </c>
+      <c r="J106">
+        <v>412</v>
+      </c>
+      <c r="K106" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.4', 'start':411, 'end':412},</v>
+      </c>
+    </row>
+    <row r="107" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H107" t="s">
+        <v>191</v>
+      </c>
+      <c r="I107">
+        <v>412</v>
+      </c>
+      <c r="J107">
+        <v>415</v>
+      </c>
+      <c r="K107" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.2.4.1', 'start':412, 'end':415},</v>
+      </c>
+    </row>
+    <row r="108" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H108" t="s">
+        <v>193</v>
+      </c>
+      <c r="I108">
+        <v>415</v>
+      </c>
+      <c r="J108">
+        <v>417</v>
+      </c>
+      <c r="K108" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.36', 'start':415, 'end':417},</v>
+      </c>
+    </row>
+    <row r="109" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H109" t="s">
+        <v>195</v>
+      </c>
+      <c r="I109">
+        <v>417</v>
+      </c>
+      <c r="J109">
+        <v>426</v>
+      </c>
+      <c r="K109" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.48', 'start':417, 'end':426},</v>
+      </c>
+    </row>
+    <row r="110" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H110" t="s">
+        <v>197</v>
+      </c>
+      <c r="I110">
+        <v>426</v>
+      </c>
+      <c r="J110">
+        <v>430</v>
+      </c>
+      <c r="K110" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.108', 'start':426, 'end':430},</v>
+      </c>
+    </row>
+    <row r="111" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H111" t="s">
+        <v>199</v>
+      </c>
+      <c r="I111">
+        <v>430</v>
+      </c>
+      <c r="J111">
+        <v>432</v>
+      </c>
+      <c r="K111" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.31', 'start':430, 'end':432},</v>
+      </c>
+    </row>
+    <row r="112" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H112" t="s">
+        <v>201</v>
+      </c>
+      <c r="I112">
+        <v>432</v>
+      </c>
+      <c r="J112">
+        <v>436</v>
+      </c>
+      <c r="K112" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.30', 'start':432, 'end':436},</v>
+      </c>
+    </row>
+    <row r="113" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H113" t="s">
+        <v>203</v>
+      </c>
+      <c r="I113">
+        <v>436</v>
+      </c>
+      <c r="J113">
+        <v>438</v>
+      </c>
+      <c r="K113" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.28', 'start':436, 'end':438},</v>
+      </c>
+    </row>
+    <row r="114" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H114" t="s">
+        <v>205</v>
+      </c>
+      <c r="I114">
+        <v>438</v>
+      </c>
+      <c r="J114">
+        <v>441</v>
+      </c>
+      <c r="K114" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.69', 'start':438, 'end':441},</v>
+      </c>
+    </row>
+    <row r="115" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H115" t="s">
+        <v>207</v>
+      </c>
+      <c r="I115">
+        <v>441</v>
+      </c>
+      <c r="J115">
+        <v>443</v>
+      </c>
+      <c r="K115" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.86', 'start':441, 'end':443},</v>
+      </c>
+    </row>
+    <row r="116" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H116" t="s">
+        <v>209</v>
+      </c>
+      <c r="I116">
+        <v>443</v>
+      </c>
+      <c r="J116">
+        <v>444</v>
+      </c>
+      <c r="K116" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.1.19', 'start':443, 'end':444},</v>
+      </c>
+    </row>
+    <row r="117" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H117" t="s">
+        <v>211</v>
+      </c>
+      <c r="I117">
+        <v>444</v>
+      </c>
+      <c r="J117">
+        <v>445</v>
+      </c>
+      <c r="K117" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.11', 'start':444, 'end':445},</v>
+      </c>
+    </row>
+    <row r="118" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H118" t="s">
+        <v>213</v>
+      </c>
+      <c r="I118">
+        <v>445</v>
+      </c>
+      <c r="J118">
+        <v>447</v>
+      </c>
+      <c r="K118" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.72', 'start':445, 'end':447},</v>
+      </c>
+    </row>
+    <row r="119" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H119" t="s">
+        <v>215</v>
+      </c>
+      <c r="I119">
+        <v>447</v>
+      </c>
+      <c r="J119">
+        <v>450</v>
+      </c>
+      <c r="K119" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.109', 'start':447, 'end':450},</v>
+      </c>
+    </row>
+    <row r="120" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H120" t="s">
+        <v>217</v>
+      </c>
+      <c r="I120">
+        <v>450</v>
+      </c>
+      <c r="J120">
+        <v>452</v>
+      </c>
+      <c r="K120" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.13', 'start':450, 'end':452},</v>
+      </c>
+    </row>
+    <row r="121" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H121" t="s">
+        <v>219</v>
+      </c>
+      <c r="I121">
+        <v>452</v>
+      </c>
+      <c r="J121">
+        <v>455</v>
+      </c>
+      <c r="K121" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.73', 'start':452, 'end':455},</v>
+      </c>
+    </row>
+    <row r="122" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H122" t="s">
+        <v>221</v>
+      </c>
+      <c r="I122">
+        <v>455</v>
+      </c>
+      <c r="J122">
+        <v>457</v>
+      </c>
+      <c r="K122" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.64', 'start':455, 'end':457},</v>
+      </c>
+    </row>
+    <row r="123" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H123" t="s">
+        <v>223</v>
+      </c>
+      <c r="I123">
+        <v>457</v>
+      </c>
+      <c r="J123">
+        <v>460</v>
+      </c>
+      <c r="K123" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.60', 'start':457, 'end':460},</v>
+      </c>
+    </row>
+    <row r="124" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H124" t="s">
+        <v>225</v>
+      </c>
+      <c r="I124">
+        <v>460</v>
+      </c>
+      <c r="J124">
+        <v>462</v>
+      </c>
+      <c r="K124" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.145', 'start':460, 'end':462},</v>
+      </c>
+    </row>
+    <row r="125" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H125" t="s">
+        <v>227</v>
+      </c>
+      <c r="I125">
+        <v>462</v>
+      </c>
+      <c r="J125">
+        <v>463</v>
+      </c>
+      <c r="K125" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.111', 'start':462, 'end':463},</v>
+      </c>
+    </row>
+    <row r="126" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H126" t="s">
+        <v>229</v>
+      </c>
+      <c r="I126">
+        <v>463</v>
+      </c>
+      <c r="J126">
+        <v>467</v>
+      </c>
+      <c r="K126" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.79', 'start':463, 'end':467},</v>
+      </c>
+    </row>
+    <row r="127" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H127" t="s">
+        <v>231</v>
+      </c>
+      <c r="I127">
+        <v>467</v>
+      </c>
+      <c r="J127">
+        <v>470</v>
+      </c>
+      <c r="K127" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.35', 'start':467, 'end':470},</v>
+      </c>
+    </row>
+    <row r="128" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H128" t="s">
+        <v>233</v>
+      </c>
+      <c r="I128">
+        <v>470</v>
+      </c>
+      <c r="J128">
+        <v>474</v>
+      </c>
+      <c r="K128" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.123', 'start':470, 'end':474},</v>
+      </c>
+    </row>
+    <row r="129" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H129" t="s">
+        <v>235</v>
+      </c>
+      <c r="I129">
+        <v>474</v>
+      </c>
+      <c r="J129">
+        <v>475</v>
+      </c>
+      <c r="K129" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.24', 'start':474, 'end':475},</v>
+      </c>
+    </row>
+    <row r="130" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H130" t="s">
+        <v>237</v>
+      </c>
+      <c r="I130">
+        <v>475</v>
+      </c>
+      <c r="J130">
+        <v>487</v>
+      </c>
+      <c r="K130" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.49', 'start':475, 'end':487},</v>
+      </c>
+    </row>
+    <row r="131" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H131" t="s">
+        <v>239</v>
+      </c>
+      <c r="I131">
+        <v>487</v>
+      </c>
+      <c r="J131">
+        <v>489</v>
+      </c>
+      <c r="K131" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.80', 'start':487, 'end':489},</v>
+      </c>
+    </row>
+    <row r="132" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H132" t="s">
+        <v>241</v>
+      </c>
+      <c r="I132">
+        <v>489</v>
+      </c>
+      <c r="J132">
+        <v>494</v>
+      </c>
+      <c r="K132" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.122', 'start':489, 'end':494},</v>
+      </c>
+    </row>
+    <row r="133" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H133" t="s">
+        <v>243</v>
+      </c>
+      <c r="I133">
+        <v>494</v>
+      </c>
+      <c r="J133">
+        <v>495</v>
+      </c>
+      <c r="K133" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.15.3.1', 'start':494, 'end':495},</v>
+      </c>
+    </row>
+    <row r="134" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H134" t="s">
+        <v>245</v>
+      </c>
+      <c r="I134">
+        <v>495</v>
+      </c>
+      <c r="J134">
+        <v>497</v>
+      </c>
+      <c r="K134" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.115', 'start':495, 'end':497},</v>
+      </c>
+    </row>
+    <row r="135" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H135" t="s">
+        <v>247</v>
+      </c>
+      <c r="I135">
+        <v>497</v>
+      </c>
+      <c r="J135">
+        <v>499</v>
+      </c>
+      <c r="K135" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.47', 'start':497, 'end':499},</v>
+      </c>
+    </row>
+    <row r="136" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H136" t="s">
+        <v>249</v>
+      </c>
+      <c r="I136">
+        <v>499</v>
+      </c>
+      <c r="J136">
+        <v>504</v>
+      </c>
+      <c r="K136" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.46', 'start':499, 'end':504},</v>
+      </c>
+    </row>
+    <row r="137" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H137" t="s">
+        <v>251</v>
+      </c>
+      <c r="I137">
+        <v>504</v>
+      </c>
+      <c r="J137">
+        <v>508</v>
+      </c>
+      <c r="K137" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.45', 'start':504, 'end':508},</v>
+      </c>
+    </row>
+    <row r="138" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H138" t="s">
+        <v>253</v>
+      </c>
+      <c r="I138">
+        <v>508</v>
+      </c>
+      <c r="J138">
+        <v>511</v>
+      </c>
+      <c r="K138" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.67', 'start':508, 'end':511},</v>
+      </c>
+    </row>
+    <row r="139" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H139" t="s">
+        <v>255</v>
+      </c>
+      <c r="I139">
+        <v>511</v>
+      </c>
+      <c r="J139">
+        <v>515</v>
+      </c>
+      <c r="K139" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.66', 'start':511, 'end':515},</v>
+      </c>
+    </row>
+    <row r="140" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H140" t="s">
+        <v>257</v>
+      </c>
+      <c r="I140">
+        <v>515</v>
+      </c>
+      <c r="J140">
+        <v>518</v>
+      </c>
+      <c r="K140" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.68', 'start':515, 'end':518},</v>
+      </c>
+    </row>
+    <row r="141" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H141" t="s">
+        <v>259</v>
+      </c>
+      <c r="I141">
+        <v>518</v>
+      </c>
+      <c r="J141">
+        <v>524</v>
+      </c>
+      <c r="K141" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.121', 'start':518, 'end':524},</v>
+      </c>
+    </row>
+    <row r="142" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H142" t="s">
+        <v>261</v>
+      </c>
+      <c r="I142">
+        <v>524</v>
+      </c>
+      <c r="J142">
+        <v>528</v>
+      </c>
+      <c r="K142" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.141', 'start':524, 'end':528},</v>
+      </c>
+    </row>
+    <row r="143" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H143" t="s">
+        <v>263</v>
+      </c>
+      <c r="I143">
+        <v>528</v>
+      </c>
+      <c r="J143">
+        <v>544</v>
+      </c>
+      <c r="K143" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.132', 'start':528, 'end':544},</v>
+      </c>
+    </row>
+    <row r="144" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H144" t="s">
+        <v>265</v>
+      </c>
+      <c r="I144">
+        <v>544</v>
+      </c>
+      <c r="J144">
+        <v>547</v>
+      </c>
+      <c r="K144" t="str">
+        <f t="shared" si="1"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.5', 'start':544, 'end':547},</v>
+      </c>
+    </row>
+    <row r="145" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H145" t="s">
+        <v>267</v>
+      </c>
+      <c r="I145">
+        <v>547</v>
+      </c>
+      <c r="J145">
+        <v>548</v>
+      </c>
+      <c r="K145" t="str">
+        <f t="shared" ref="K145:K208" si="2">"{ 'index':'"&amp;H145&amp;"', 'start':"&amp;I145&amp;", 'end':"&amp;J145&amp;"},"</f>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.77', 'start':547, 'end':548},</v>
+      </c>
+    </row>
+    <row r="146" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H146" t="s">
+        <v>269</v>
+      </c>
+      <c r="I146">
+        <v>548</v>
+      </c>
+      <c r="J146">
+        <v>550</v>
+      </c>
+      <c r="K146" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.34', 'start':548, 'end':550},</v>
+      </c>
+    </row>
+    <row r="147" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H147" t="s">
+        <v>271</v>
+      </c>
+      <c r="I147">
+        <v>550</v>
+      </c>
+      <c r="J147">
+        <v>553</v>
+      </c>
+      <c r="K147" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.33', 'start':550, 'end':553},</v>
+      </c>
+    </row>
+    <row r="148" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H148" t="s">
+        <v>273</v>
+      </c>
+      <c r="I148">
+        <v>553</v>
+      </c>
+      <c r="J148">
+        <v>567</v>
+      </c>
+      <c r="K148" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.52', 'start':553, 'end':567},</v>
+      </c>
+    </row>
+    <row r="149" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H149" t="s">
+        <v>275</v>
+      </c>
+      <c r="I149">
+        <v>567</v>
+      </c>
+      <c r="J149">
+        <v>573</v>
+      </c>
+      <c r="K149" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.54', 'start':567, 'end':573},</v>
+      </c>
+    </row>
+    <row r="150" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H150" t="s">
+        <v>277</v>
+      </c>
+      <c r="I150">
+        <v>573</v>
+      </c>
+      <c r="J150">
+        <v>575</v>
+      </c>
+      <c r="K150" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.53', 'start':573, 'end':575},</v>
+      </c>
+    </row>
+    <row r="151" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H151" t="s">
+        <v>279</v>
+      </c>
+      <c r="I151">
+        <v>575</v>
+      </c>
+      <c r="J151">
+        <v>578</v>
+      </c>
+      <c r="K151" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.19', 'start':575, 'end':578},</v>
+      </c>
+    </row>
+    <row r="152" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H152" t="s">
+        <v>281</v>
+      </c>
+      <c r="I152">
+        <v>578</v>
+      </c>
+      <c r="J152">
+        <v>581</v>
+      </c>
+      <c r="K152" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.20', 'start':578, 'end':581},</v>
+      </c>
+    </row>
+    <row r="153" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H153" t="s">
+        <v>283</v>
+      </c>
+      <c r="I153">
+        <v>581</v>
+      </c>
+      <c r="J153">
+        <v>590</v>
+      </c>
+      <c r="K153" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.131', 'start':581, 'end':590},</v>
+      </c>
+    </row>
+    <row r="154" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H154" t="s">
+        <v>651</v>
+      </c>
+      <c r="I154">
+        <v>590</v>
+      </c>
+      <c r="J154">
+        <v>594</v>
+      </c>
+      <c r="K154" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.135', 'start':590, 'end':594},</v>
+      </c>
+    </row>
+    <row r="155" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H155" t="s">
+        <v>286</v>
+      </c>
+      <c r="I155">
+        <v>594</v>
+      </c>
+      <c r="J155">
+        <v>604</v>
+      </c>
+      <c r="K155" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.16', 'start':594, 'end':604},</v>
+      </c>
+    </row>
+    <row r="156" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H156" t="s">
+        <v>288</v>
+      </c>
+      <c r="I156">
+        <v>604</v>
+      </c>
+      <c r="J156">
+        <v>607</v>
+      </c>
+      <c r="K156" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.18', 'start':604, 'end':607},</v>
+      </c>
+    </row>
+    <row r="157" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H157" t="s">
+        <v>290</v>
+      </c>
+      <c r="I157">
+        <v>607</v>
+      </c>
+      <c r="J157">
+        <v>609</v>
+      </c>
+      <c r="K157" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.147', 'start':607, 'end':609},</v>
+      </c>
+    </row>
+    <row r="158" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H158" t="s">
+        <v>292</v>
+      </c>
+      <c r="I158">
+        <v>609</v>
+      </c>
+      <c r="J158">
+        <v>617</v>
+      </c>
+      <c r="K158" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.23', 'start':609, 'end':617},</v>
+      </c>
+    </row>
+    <row r="159" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H159" t="s">
+        <v>294</v>
+      </c>
+      <c r="I159">
+        <v>617</v>
+      </c>
+      <c r="J159">
+        <v>620</v>
+      </c>
+      <c r="K159" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.17', 'start':617, 'end':620},</v>
+      </c>
+    </row>
+    <row r="160" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H160" t="s">
+        <v>296</v>
+      </c>
+      <c r="I160">
+        <v>620</v>
+      </c>
+      <c r="J160">
+        <v>625</v>
+      </c>
+      <c r="K160" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.74', 'start':620, 'end':625},</v>
+      </c>
+    </row>
+    <row r="161" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H161" t="s">
+        <v>298</v>
+      </c>
+      <c r="I161">
+        <v>625</v>
+      </c>
+      <c r="J161">
+        <v>628</v>
+      </c>
+      <c r="K161" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.75', 'start':625, 'end':628},</v>
+      </c>
+    </row>
+    <row r="162" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H162" t="s">
+        <v>300</v>
+      </c>
+      <c r="I162">
+        <v>628</v>
+      </c>
+      <c r="J162">
+        <v>631</v>
+      </c>
+      <c r="K162" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.50', 'start':628, 'end':631},</v>
+      </c>
+    </row>
+    <row r="163" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H163" t="s">
+        <v>302</v>
+      </c>
+      <c r="I163">
+        <v>631</v>
+      </c>
+      <c r="J163">
+        <v>635</v>
+      </c>
+      <c r="K163" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.76', 'start':631, 'end':635},</v>
+      </c>
+    </row>
+    <row r="164" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H164" t="s">
+        <v>304</v>
+      </c>
+      <c r="I164">
+        <v>635</v>
+      </c>
+      <c r="J164">
+        <v>638</v>
+      </c>
+      <c r="K164" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.138', 'start':635, 'end':638},</v>
+      </c>
+    </row>
+    <row r="165" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H165" t="s">
+        <v>652</v>
+      </c>
+      <c r="I165">
+        <v>638</v>
+      </c>
+      <c r="J165">
+        <v>643</v>
+      </c>
+      <c r="K165" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.130', 'start':638, 'end':643},</v>
+      </c>
+    </row>
+    <row r="166" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H166" t="s">
+        <v>307</v>
+      </c>
+      <c r="I166">
+        <v>643</v>
+      </c>
+      <c r="J166">
+        <v>647</v>
+      </c>
+      <c r="K166" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.124', 'start':643, 'end':647},</v>
+      </c>
+    </row>
+    <row r="167" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H167" t="s">
+        <v>309</v>
+      </c>
+      <c r="I167">
+        <v>647</v>
+      </c>
+      <c r="J167">
+        <v>651</v>
+      </c>
+      <c r="K167" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.144', 'start':647, 'end':651},</v>
+      </c>
+    </row>
+    <row r="168" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H168" t="s">
+        <v>311</v>
+      </c>
+      <c r="I168">
+        <v>651</v>
+      </c>
+      <c r="J168">
+        <v>660</v>
+      </c>
+      <c r="K168" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.140', 'start':651, 'end':660},</v>
+      </c>
+    </row>
+    <row r="169" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H169" t="s">
+        <v>313</v>
+      </c>
+      <c r="I169">
+        <v>660</v>
+      </c>
+      <c r="J169">
+        <v>663</v>
+      </c>
+      <c r="K169" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.39', 'start':660, 'end':663},</v>
+      </c>
+    </row>
+    <row r="170" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H170" t="s">
+        <v>315</v>
+      </c>
+      <c r="I170">
+        <v>663</v>
+      </c>
+      <c r="J170">
+        <v>667</v>
+      </c>
+      <c r="K170" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.129', 'start':663, 'end':667},</v>
+      </c>
+    </row>
+    <row r="171" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H171" t="s">
+        <v>317</v>
+      </c>
+      <c r="I171">
+        <v>667</v>
+      </c>
+      <c r="J171">
+        <v>671</v>
+      </c>
+      <c r="K171" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.40', 'start':667, 'end':671},</v>
+      </c>
+    </row>
+    <row r="172" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H172" t="s">
+        <v>319</v>
+      </c>
+      <c r="I172">
+        <v>671</v>
+      </c>
+      <c r="J172">
+        <v>677</v>
+      </c>
+      <c r="K172" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.120', 'start':671, 'end':677},</v>
+      </c>
+    </row>
+    <row r="173" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H173" t="s">
+        <v>321</v>
+      </c>
+      <c r="I173">
+        <v>677</v>
+      </c>
+      <c r="J173">
+        <v>686</v>
+      </c>
+      <c r="K173" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.146', 'start':677, 'end':686},</v>
+      </c>
+    </row>
+    <row r="174" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H174" t="s">
+        <v>323</v>
+      </c>
+      <c r="I174">
+        <v>686</v>
+      </c>
+      <c r="J174">
+        <v>692</v>
+      </c>
+      <c r="K174" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.42', 'start':686, 'end':692},</v>
+      </c>
+    </row>
+    <row r="175" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H175" t="s">
+        <v>325</v>
+      </c>
+      <c r="I175">
+        <v>692</v>
+      </c>
+      <c r="J175">
+        <v>697</v>
+      </c>
+      <c r="K175" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.44', 'start':692, 'end':697},</v>
+      </c>
+    </row>
+    <row r="176" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H176" t="s">
+        <v>327</v>
+      </c>
+      <c r="I176">
+        <v>697</v>
+      </c>
+      <c r="J176">
+        <v>703</v>
+      </c>
+      <c r="K176" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.41', 'start':697, 'end':703},</v>
+      </c>
+    </row>
+    <row r="177" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H177" t="s">
+        <v>329</v>
+      </c>
+      <c r="I177">
+        <v>703</v>
+      </c>
+      <c r="J177">
+        <v>709</v>
+      </c>
+      <c r="K177" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.43', 'start':703, 'end':709},</v>
+      </c>
+    </row>
+    <row r="178" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H178" t="s">
+        <v>331</v>
+      </c>
+      <c r="I178">
+        <v>709</v>
+      </c>
+      <c r="J178">
+        <v>721</v>
+      </c>
+      <c r="K178" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.61', 'start':709, 'end':721},</v>
+      </c>
+    </row>
+    <row r="179" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H179" t="s">
+        <v>333</v>
+      </c>
+      <c r="I179">
+        <v>721</v>
+      </c>
+      <c r="J179">
+        <v>723</v>
+      </c>
+      <c r="K179" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.51', 'start':721, 'end':723},</v>
+      </c>
+    </row>
+    <row r="180" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H180" t="s">
+        <v>335</v>
+      </c>
+      <c r="I180">
+        <v>723</v>
+      </c>
+      <c r="J180">
+        <v>725</v>
+      </c>
+      <c r="K180" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.25', 'start':723, 'end':725},</v>
+      </c>
+    </row>
+    <row r="181" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H181" t="s">
+        <v>337</v>
+      </c>
+      <c r="I181">
+        <v>725</v>
+      </c>
+      <c r="J181">
+        <v>727</v>
+      </c>
+      <c r="K181" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.15.3.8', 'start':725, 'end':727},</v>
+      </c>
+    </row>
+    <row r="182" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H182" t="s">
+        <v>339</v>
+      </c>
+      <c r="I182">
+        <v>727</v>
+      </c>
+      <c r="J182">
+        <v>729</v>
+      </c>
+      <c r="K182" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.65', 'start':727, 'end':729},</v>
+      </c>
+    </row>
+    <row r="183" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H183" t="s">
+        <v>341</v>
+      </c>
+      <c r="I183">
+        <v>729</v>
+      </c>
+      <c r="J183">
+        <v>735</v>
+      </c>
+      <c r="K183" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.70', 'start':729, 'end':735},</v>
+      </c>
+    </row>
+    <row r="184" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H184" t="s">
+        <v>343</v>
+      </c>
+      <c r="I184">
+        <v>735</v>
+      </c>
+      <c r="J184">
+        <v>738</v>
+      </c>
+      <c r="K184" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.143', 'start':735, 'end':738},</v>
+      </c>
+    </row>
+    <row r="185" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H185" t="s">
+        <v>345</v>
+      </c>
+      <c r="I185">
+        <v>738</v>
+      </c>
+      <c r="J185">
+        <v>743</v>
+      </c>
+      <c r="K185" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.3', 'start':738, 'end':743},</v>
+      </c>
+    </row>
+    <row r="186" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H186" t="s">
+        <v>347</v>
+      </c>
+      <c r="I186">
+        <v>743</v>
+      </c>
+      <c r="J186">
+        <v>750</v>
+      </c>
+      <c r="K186" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.4', 'start':743, 'end':750},</v>
+      </c>
+    </row>
+    <row r="187" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H187" t="s">
+        <v>349</v>
+      </c>
+      <c r="I187">
+        <v>750</v>
+      </c>
+      <c r="J187">
+        <v>756</v>
+      </c>
+      <c r="K187" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.114', 'start':750, 'end':756},</v>
+      </c>
+    </row>
+    <row r="188" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H188" t="s">
+        <v>351</v>
+      </c>
+      <c r="I188">
+        <v>756</v>
+      </c>
+      <c r="J188">
+        <v>758</v>
+      </c>
+      <c r="K188" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.6', 'start':756, 'end':758},</v>
+      </c>
+    </row>
+    <row r="189" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H189" t="s">
+        <v>353</v>
+      </c>
+      <c r="I189">
+        <v>758</v>
+      </c>
+      <c r="J189">
+        <v>765</v>
+      </c>
+      <c r="K189" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.12', 'start':758, 'end':765},</v>
+      </c>
+    </row>
+    <row r="190" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H190" t="s">
+        <v>355</v>
+      </c>
+      <c r="I190">
+        <v>765</v>
+      </c>
+      <c r="J190">
+        <v>772</v>
+      </c>
+      <c r="K190" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.13', 'start':765, 'end':772},</v>
+      </c>
+    </row>
+    <row r="191" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H191" t="s">
+        <v>357</v>
+      </c>
+      <c r="I191">
+        <v>772</v>
+      </c>
+      <c r="J191">
+        <v>779</v>
+      </c>
+      <c r="K191" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.14', 'start':772, 'end':779},</v>
+      </c>
+    </row>
+    <row r="192" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H192" t="s">
+        <v>359</v>
+      </c>
+      <c r="I192">
+        <v>779</v>
+      </c>
+      <c r="J192">
+        <v>781</v>
+      </c>
+      <c r="K192" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.5', 'start':779, 'end':781},</v>
+      </c>
+    </row>
+    <row r="193" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H193" t="s">
+        <v>361</v>
+      </c>
+      <c r="I193">
+        <v>781</v>
+      </c>
+      <c r="J193">
+        <v>783</v>
+      </c>
+      <c r="K193" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.37', 'start':781, 'end':783},</v>
+      </c>
+    </row>
+    <row r="194" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H194" t="s">
+        <v>363</v>
+      </c>
+      <c r="I194">
+        <v>783</v>
+      </c>
+      <c r="J194">
+        <v>785</v>
+      </c>
+      <c r="K194" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.113', 'start':783, 'end':785},</v>
+      </c>
+    </row>
+    <row r="195" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H195" t="s">
+        <v>365</v>
+      </c>
+      <c r="I195">
+        <v>785</v>
+      </c>
+      <c r="J195">
+        <v>787</v>
+      </c>
+      <c r="K195" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.110', 'start':785, 'end':787},</v>
+      </c>
+    </row>
+    <row r="196" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H196" t="s">
+        <v>367</v>
+      </c>
+      <c r="I196">
+        <v>787</v>
+      </c>
+      <c r="J196">
+        <v>789</v>
+      </c>
+      <c r="K196" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.9', 'start':787, 'end':789},</v>
+      </c>
+    </row>
+    <row r="197" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H197" t="s">
+        <v>369</v>
+      </c>
+      <c r="I197">
+        <v>789</v>
+      </c>
+      <c r="J197">
+        <v>793</v>
+      </c>
+      <c r="K197" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.14', 'start':789, 'end':793},</v>
+      </c>
+    </row>
+    <row r="198" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H198" t="s">
+        <v>371</v>
+      </c>
+      <c r="I198">
+        <v>793</v>
+      </c>
+      <c r="J198">
+        <v>797</v>
+      </c>
+      <c r="K198" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.9', 'start':793, 'end':797},</v>
+      </c>
+    </row>
+    <row r="199" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H199" t="s">
+        <v>373</v>
+      </c>
+      <c r="I199">
+        <v>797</v>
+      </c>
+      <c r="J199">
+        <v>798</v>
+      </c>
+      <c r="K199" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.10', 'start':797, 'end':798},</v>
+      </c>
+    </row>
+    <row r="200" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H200" t="s">
+        <v>375</v>
+      </c>
+      <c r="I200">
+        <v>798</v>
+      </c>
+      <c r="J200">
+        <v>803</v>
+      </c>
+      <c r="K200" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.2', 'start':798, 'end':803},</v>
+      </c>
+    </row>
+    <row r="201" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H201" t="s">
+        <v>377</v>
+      </c>
+      <c r="I201">
+        <v>803</v>
+      </c>
+      <c r="J201">
+        <v>807</v>
+      </c>
+      <c r="K201" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.1', 'start':803, 'end':807},</v>
+      </c>
+    </row>
+    <row r="202" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H202" t="s">
+        <v>379</v>
+      </c>
+      <c r="I202">
+        <v>807</v>
+      </c>
+      <c r="J202">
+        <v>823</v>
+      </c>
+      <c r="K202" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.136', 'start':807, 'end':823},</v>
+      </c>
+    </row>
+    <row r="203" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H203" t="s">
+        <v>381</v>
+      </c>
+      <c r="I203">
+        <v>823</v>
+      </c>
+      <c r="J203">
+        <v>826</v>
+      </c>
+      <c r="K203" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.128', 'start':823, 'end':826},</v>
+      </c>
+    </row>
+    <row r="204" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H204" t="s">
+        <v>383</v>
+      </c>
+      <c r="I204">
+        <v>826</v>
+      </c>
+      <c r="J204">
+        <v>831</v>
+      </c>
+      <c r="K204" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.127', 'start':826, 'end':831},</v>
+      </c>
+    </row>
+    <row r="205" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H205" t="s">
+        <v>385</v>
+      </c>
+      <c r="I205">
+        <v>831</v>
+      </c>
+      <c r="J205">
+        <v>834</v>
+      </c>
+      <c r="K205" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.63', 'start':831, 'end':834},</v>
+      </c>
+    </row>
+    <row r="206" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H206" t="s">
+        <v>387</v>
+      </c>
+      <c r="I206">
+        <v>834</v>
+      </c>
+      <c r="J206">
+        <v>837</v>
+      </c>
+      <c r="K206" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.32', 'start':834, 'end':837},</v>
+      </c>
+    </row>
+    <row r="207" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H207" t="s">
+        <v>389</v>
+      </c>
+      <c r="I207">
+        <v>837</v>
+      </c>
+      <c r="J207">
+        <v>840</v>
+      </c>
+      <c r="K207" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.8', 'start':837, 'end':840},</v>
+      </c>
+    </row>
+    <row r="208" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H208" t="s">
+        <v>391</v>
+      </c>
+      <c r="I208">
+        <v>840</v>
+      </c>
+      <c r="J208">
+        <v>844</v>
+      </c>
+      <c r="K208" t="str">
+        <f t="shared" si="2"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.78', 'start':840, 'end':844},</v>
+      </c>
+    </row>
+    <row r="209" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H209" t="s">
+        <v>393</v>
+      </c>
+      <c r="I209">
+        <v>844</v>
+      </c>
+      <c r="J209">
+        <v>848</v>
+      </c>
+      <c r="K209" t="str">
+        <f t="shared" ref="K209:K230" si="3">"{ 'index':'"&amp;H209&amp;"', 'start':"&amp;I209&amp;", 'end':"&amp;J209&amp;"},"</f>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.38', 'start':844, 'end':848},</v>
+      </c>
+    </row>
+    <row r="210" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H210" t="s">
+        <v>395</v>
+      </c>
+      <c r="I210">
+        <v>848</v>
+      </c>
+      <c r="J210">
+        <v>851</v>
+      </c>
+      <c r="K210" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.8', 'start':848, 'end':851},</v>
+      </c>
+    </row>
+    <row r="211" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H211" t="s">
+        <v>397</v>
+      </c>
+      <c r="I211">
+        <v>851</v>
+      </c>
+      <c r="J211">
+        <v>853</v>
+      </c>
+      <c r="K211" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.6', 'start':851, 'end':853},</v>
+      </c>
+    </row>
+    <row r="212" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H212" t="s">
+        <v>399</v>
+      </c>
+      <c r="I212">
+        <v>853</v>
+      </c>
+      <c r="J212">
+        <v>855</v>
+      </c>
+      <c r="K212" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.118', 'start':853, 'end':855},</v>
+      </c>
+    </row>
+    <row r="213" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H213" t="s">
+        <v>401</v>
+      </c>
+      <c r="I213">
+        <v>855</v>
+      </c>
+      <c r="J213">
+        <v>862</v>
+      </c>
+      <c r="K213" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.24.3.90', 'start':855, 'end':862},</v>
+      </c>
+    </row>
+    <row r="214" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H214" t="s">
+        <v>403</v>
+      </c>
+      <c r="I214">
+        <v>862</v>
+      </c>
+      <c r="J214">
+        <v>868</v>
+      </c>
+      <c r="K214" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.7', 'start':862, 'end':868},</v>
+      </c>
+    </row>
+    <row r="215" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H215" t="s">
+        <v>405</v>
+      </c>
+      <c r="I215">
+        <v>868</v>
+      </c>
+      <c r="J215">
+        <v>871</v>
+      </c>
+      <c r="K215" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.12', 'start':868, 'end':871},</v>
+      </c>
+    </row>
+    <row r="216" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H216" t="s">
+        <v>407</v>
+      </c>
+      <c r="I216">
+        <v>871</v>
+      </c>
+      <c r="J216">
+        <v>875</v>
+      </c>
+      <c r="K216" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.85', 'start':871, 'end':875},</v>
+      </c>
+    </row>
+    <row r="217" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H217" t="s">
+        <v>409</v>
+      </c>
+      <c r="I217">
+        <v>875</v>
+      </c>
+      <c r="J217">
+        <v>879</v>
+      </c>
+      <c r="K217" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.27', 'start':875, 'end':879},</v>
+      </c>
+    </row>
+    <row r="218" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H218" t="s">
+        <v>411</v>
+      </c>
+      <c r="I218">
+        <v>879</v>
+      </c>
+      <c r="J218">
+        <v>883</v>
+      </c>
+      <c r="K218" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.26', 'start':879, 'end':883},</v>
+      </c>
+    </row>
+    <row r="219" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H219" t="s">
+        <v>413</v>
+      </c>
+      <c r="I219">
+        <v>883</v>
+      </c>
+      <c r="J219">
+        <v>885</v>
+      </c>
+      <c r="K219" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.134', 'start':883, 'end':885},</v>
+      </c>
+    </row>
+    <row r="220" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H220" t="s">
+        <v>653</v>
+      </c>
+      <c r="I220">
+        <v>885</v>
+      </c>
+      <c r="J220">
+        <v>888</v>
+      </c>
+      <c r="K220" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.133', 'start':885, 'end':888},</v>
+      </c>
+    </row>
+    <row r="221" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H221" t="s">
+        <v>6</v>
+      </c>
+      <c r="I221">
+        <v>41</v>
+      </c>
+      <c r="J221">
+        <v>87</v>
+      </c>
+      <c r="K221" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.1.1', 'start':41, 'end':87},</v>
+      </c>
+    </row>
+    <row r="222" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H222" t="s">
+        <v>32</v>
+      </c>
+      <c r="I222">
+        <v>233</v>
+      </c>
+      <c r="J222">
+        <v>255</v>
+      </c>
+      <c r="K222" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.29.1', 'start':233, 'end':255},</v>
+      </c>
+    </row>
+    <row r="223" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H223" t="s">
+        <v>416</v>
+      </c>
+      <c r="I223">
+        <v>888</v>
+      </c>
+      <c r="J223">
+        <v>892</v>
+      </c>
+      <c r="K223" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.4.119', 'start':888, 'end':892},</v>
+      </c>
+    </row>
+    <row r="224" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H224" t="s">
+        <v>418</v>
+      </c>
+      <c r="I224">
+        <v>892</v>
+      </c>
+      <c r="J224">
+        <v>894</v>
+      </c>
+      <c r="K224" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.2', 'start':892, 'end':894},</v>
+      </c>
+    </row>
+    <row r="225" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H225" t="s">
+        <v>420</v>
+      </c>
+      <c r="I225">
+        <v>894</v>
+      </c>
+      <c r="J225">
+        <v>896</v>
+      </c>
+      <c r="K225" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.6.2.1', 'start':894, 'end':896},</v>
+      </c>
+    </row>
+    <row r="226" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H226" t="s">
+        <v>422</v>
+      </c>
+      <c r="I226">
+        <v>896</v>
+      </c>
+      <c r="J226">
+        <v>900</v>
+      </c>
+      <c r="K226" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.5.2', 'start':896, 'end':900},</v>
+      </c>
+    </row>
+    <row r="227" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H227" t="s">
+        <v>424</v>
+      </c>
+      <c r="I227">
+        <v>900</v>
+      </c>
+      <c r="J227">
+        <v>900</v>
+      </c>
+      <c r="K227" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.5.3', 'start':900, 'end':900},</v>
+      </c>
+    </row>
+    <row r="228" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H228" t="s">
+        <v>426</v>
+      </c>
+      <c r="I228">
+        <v>900</v>
+      </c>
+      <c r="J228">
+        <v>901</v>
+      </c>
+      <c r="K228" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.5.4', 'start':900, 'end':901},</v>
+      </c>
+    </row>
+    <row r="229" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H229" t="s">
+        <v>428</v>
+      </c>
+      <c r="I229">
+        <v>901</v>
+      </c>
+      <c r="J229">
+        <v>904</v>
+      </c>
+      <c r="K229" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.5.1', 'start':901, 'end':904},</v>
+      </c>
+    </row>
+    <row r="230" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H230" t="s">
+        <v>430</v>
+      </c>
+      <c r="I230">
+        <v>904</v>
+      </c>
+      <c r="J230">
+        <v>904</v>
+      </c>
+      <c r="K230" t="str">
+        <f t="shared" si="3"/>
+        <v>{ 'index':'2.16.840.1.113883.10.20.22.5.1.1', 'start':904, 'end':904},</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CDA-20551 and fix associated index
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnD'Amore\Source\Repos\ccda-search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0AE666-4AA4-492C-8054-AE7809B41C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3977121-4CEC-4600-A9DA-1B81A36A9C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4784" uniqueCount="1923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4784" uniqueCount="1924">
   <si>
     <t>Template_Type</t>
   </si>
@@ -5807,6 +5807,9 @@
   </si>
   <si>
     <t>Indication  (Companion Guide)</t>
+  </si>
+  <si>
+    <t>Reaction Observation (Companion Guide)</t>
   </si>
 </sst>
 </file>
@@ -6756,8 +6759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B158" sqref="B158"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B212" sqref="B212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15055,7 +15058,7 @@
         <v>1918</v>
       </c>
       <c r="K194" t="str">
-        <f t="shared" ref="K194:K257" si="12">B194&amp;" "&amp;D194&amp;" "&amp;J194</f>
+        <f t="shared" ref="K194:K252" si="12">B194&amp;" "&amp;D194&amp;" "&amp;J194</f>
         <v>Pregnancy Intention in Next Year (Companion Guide) 2.16.840.1.113883.10.20.22.4.281 CONF:4537-26557;CONF:4537-26558;CONF:4537-26549;CONF:4537-26552;CONF:4537-26553;CONF:4537-26981;CONF:4537-26550;CONF:4537-26554;CONF:4537-26555;CONF:4537-26551;CONF:4537-26556;CONF:4537-26560;CONF:4537-26821;CONF:4537-26822;CONF:4537-26559;</v>
       </c>
       <c r="M194" t="str">
@@ -15764,7 +15767,7 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>370</v>
+        <v>1923</v>
       </c>
       <c r="C211" t="s">
         <v>432</v>
@@ -15790,11 +15793,11 @@
       </c>
       <c r="K211" t="str">
         <f t="shared" si="12"/>
-        <v>Reaction Observation   2.16.840.1.113883.10.20.22.4.9 CONF:1098-7325;CONF:1098-7326;CONF:1098-7323;CONF:1098-10523;CONF:1098-32504;CONF:1098-7329;CONF:1098-16851;CONF:1098-31124;CONF:1098-32169;CONF:1098-7328;CONF:1098-19114;CONF:1098-7332;CONF:1098-7333;CONF:1098-7334;CONF:1098-7335;CONF:1098-7337;CONF:1098-7338;CONF:1098-7343;CONF:1098-15920;CONF:1098-7340;CONF:1098-7341;CONF:1098-7344;CONF:1098-15921;CONF:1098-7580;CONF:1098-7581;CONF:1098-10375;CONF:1098-15922</v>
+        <v>Reaction Observation (Companion Guide) 2.16.840.1.113883.10.20.22.4.9 CONF:1098-7325;CONF:1098-7326;CONF:1098-7323;CONF:1098-10523;CONF:1098-32504;CONF:1098-7329;CONF:1098-16851;CONF:1098-31124;CONF:1098-32169;CONF:1098-7328;CONF:1098-19114;CONF:1098-7332;CONF:1098-7333;CONF:1098-7334;CONF:1098-7335;CONF:1098-7337;CONF:1098-7338;CONF:1098-7343;CONF:1098-15920;CONF:1098-7340;CONF:1098-7341;CONF:1098-7344;CONF:1098-15921;CONF:1098-7580;CONF:1098-7581;CONF:1098-10375;CONF:1098-15922</v>
       </c>
       <c r="M211" t="str">
         <f t="shared" si="13"/>
-        <v>{ 'id': '210', 'template_type': 'Entry', 'name': 'Reaction Observation   [2.16.840.1.113883.10.20.22.4.9[793-797', 'name2': 'Reaction Observation  ', 'template': '2.16.840.1.113883.10.20.22.4.9', 'pageStart': '793', 'pages': '793-797', 'search': 'Reaction Observation   2.16.840.1.113883.10.20.22.4.9 CONF:1098-7325;CONF:1098-7326;CONF:1098-7323;CONF:1098-10523;CONF:1098-32504;CONF:1098-7329;CONF:1098-16851;CONF:1098-31124;CONF:1098-32169;CONF:1098-7328;CONF:1098-19114;CONF:1098-7332;CONF:1098-7333;CONF:1098-7334;CONF:1098-7335;CONF:1098-7337;CONF:1098-7338;CONF:1098-7343;CONF:1098-15920;CONF:1098-7340;CONF:1098-7341;CONF:1098-7344;CONF:1098-15921;CONF:1098-7580;CONF:1098-7581;CONF:1098-10375;CONF:1098-15922' },</v>
+        <v>{ 'id': '210', 'template_type': 'Entry', 'name': 'Reaction Observation (Companion Guide) [2.16.840.1.113883.10.20.22.4.9[793-797', 'name2': 'Reaction Observation (Companion Guide)', 'template': '2.16.840.1.113883.10.20.22.4.9', 'pageStart': '793', 'pages': '793-797', 'search': 'Reaction Observation (Companion Guide) 2.16.840.1.113883.10.20.22.4.9 CONF:1098-7325;CONF:1098-7326;CONF:1098-7323;CONF:1098-10523;CONF:1098-32504;CONF:1098-7329;CONF:1098-16851;CONF:1098-31124;CONF:1098-32169;CONF:1098-7328;CONF:1098-19114;CONF:1098-7332;CONF:1098-7333;CONF:1098-7334;CONF:1098-7335;CONF:1098-7337;CONF:1098-7338;CONF:1098-7343;CONF:1098-15920;CONF:1098-7340;CONF:1098-7341;CONF:1098-7344;CONF:1098-15921;CONF:1098-7580;CONF:1098-7581;CONF:1098-10375;CONF:1098-15922' },</v>
       </c>
       <c r="N211" t="str">
         <f t="shared" si="14"/>
@@ -15899,11 +15902,14 @@
         <v>375</v>
       </c>
       <c r="E214">
-        <v>798</v>
-      </c>
-      <c r="G214" s="3" t="str">
-        <f>VLOOKUP(D214,'2022_New_Pages'!$H$1:$I$215,2,0)</f>
-        <v>798-803</v>
+        <v>1200</v>
+      </c>
+      <c r="F214">
+        <v>1207</v>
+      </c>
+      <c r="G214" t="str">
+        <f>"CG_A_"&amp;E214-1000&amp;"-"&amp;F214-1000</f>
+        <v>CG_A_200-207</v>
       </c>
       <c r="H214" t="s">
         <v>894</v>
@@ -15920,7 +15926,7 @@
       </c>
       <c r="M214" t="str">
         <f t="shared" si="13"/>
-        <v>{ 'id': '213', 'template_type': 'Entry', 'name': 'Result Observation  [2.16.840.1.113883.10.20.22.4.2[798-803', 'name2': 'Result Observation ', 'template': '2.16.840.1.113883.10.20.22.4.2', 'pageStart': '798', 'pages': '798-803', 'search': 'Result Observation  2.16.840.1.113883.10.20.22.4.2 CONF:1198-7130;CONF:1198-7131;CONF:1198-7136;CONF:1198-9138;CONF:1198-32575;CONF:1198-7137;CONF:1198-7133;CONF:1198-19212;CONF:1198-7134;CONF:1198-14849;CONF:1198-7140;CONF:1198-7143;CONF:1198-31484;CONF:1198-31866;CONF:1198-32610;CONF:1198-7147;CONF:1198-32476;CONF:1198-7148;CONF:1198-7153;CONF:1198-7149;CONF:1198-7150;CONF:1198-7151;CONF:1198-7152;CONF:1198-32175' },</v>
+        <v>{ 'id': '213', 'template_type': 'Entry', 'name': 'Result Observation  [2.16.840.1.113883.10.20.22.4.2[CG_A_200-207', 'name2': 'Result Observation ', 'template': '2.16.840.1.113883.10.20.22.4.2', 'pageStart': '1200', 'pages': 'CG_A_200-207', 'search': 'Result Observation  2.16.840.1.113883.10.20.22.4.2 CONF:1198-7130;CONF:1198-7131;CONF:1198-7136;CONF:1198-9138;CONF:1198-32575;CONF:1198-7137;CONF:1198-7133;CONF:1198-19212;CONF:1198-7134;CONF:1198-14849;CONF:1198-7140;CONF:1198-7143;CONF:1198-31484;CONF:1198-31866;CONF:1198-32610;CONF:1198-7147;CONF:1198-32476;CONF:1198-7148;CONF:1198-7153;CONF:1198-7149;CONF:1198-7150;CONF:1198-7151;CONF:1198-7152;CONF:1198-32175' },</v>
       </c>
       <c r="N214" t="str">
         <f t="shared" si="14"/>
@@ -15942,14 +15948,14 @@
         <v>377</v>
       </c>
       <c r="E215">
-        <v>1200</v>
+        <v>1207</v>
       </c>
       <c r="F215">
-        <v>1207</v>
+        <v>1211</v>
       </c>
       <c r="G215" t="str">
         <f>"CG_A_"&amp;E215-1000&amp;"-"&amp;F215-1000</f>
-        <v>CG_A_200-207</v>
+        <v>CG_A_207-211</v>
       </c>
       <c r="H215" t="s">
         <v>895</v>
@@ -15966,7 +15972,7 @@
       </c>
       <c r="M215" t="str">
         <f t="shared" si="13"/>
-        <v>{ 'id': '214', 'template_type': 'Entry', 'name': 'Result Organizer (Companion Guide) [2.16.840.1.113883.10.20.22.4.1[CG_A_200-207', 'name2': 'Result Organizer (Companion Guide)', 'template': '2.16.840.1.113883.10.20.22.4.1', 'pageStart': '1200', 'pages': 'CG_A_200-207', 'search': 'Result Organizer (Companion Guide) 2.16.840.1.113883.10.20.22.4.1 CONF:1198-7121;CONF:1198-7122;CONF:1198-7126;CONF:1198-9134;CONF:1198-32588;CONF:1198-7127;CONF:1198-7128;CONF:1198-19218;CONF:1198-19219;CONF:1198-7123;CONF:1198-14848;CONF:1198-31865;CONF:1198-32488;CONF:1198-32489;CONF:1198-31149;CONF:1198-7124;CONF:1198-14850' },</v>
+        <v>{ 'id': '214', 'template_type': 'Entry', 'name': 'Result Organizer (Companion Guide) [2.16.840.1.113883.10.20.22.4.1[CG_A_207-211', 'name2': 'Result Organizer (Companion Guide)', 'template': '2.16.840.1.113883.10.20.22.4.1', 'pageStart': '1207', 'pages': 'CG_A_207-211', 'search': 'Result Organizer (Companion Guide) 2.16.840.1.113883.10.20.22.4.1 CONF:1198-7121;CONF:1198-7122;CONF:1198-7126;CONF:1198-9134;CONF:1198-32588;CONF:1198-7127;CONF:1198-7128;CONF:1198-19218;CONF:1198-19219;CONF:1198-7123;CONF:1198-14848;CONF:1198-31865;CONF:1198-32488;CONF:1198-32489;CONF:1198-31149;CONF:1198-7124;CONF:1198-14850' },</v>
       </c>
       <c r="N215" t="str">
         <f t="shared" si="14"/>

</xml_diff>